<commit_message>
Calibrate ETS for split between onshore and offshore wind
</commit_message>
<xml_diff>
--- a/InputData/elec/ETS/Electricity Technology Shareweights.xlsx
+++ b/InputData/elec/ETS/Electricity Technology Shareweights.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-eu\InputData\elec\ETS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-eu\InputData\elec\ETS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CA3800-5A2B-4C7A-8CED-01AD04BCD2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="ETS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -192,7 +193,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -575,21 +576,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -597,84 +598,84 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1"/>
+    <hyperlink ref="A8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -682,22 +683,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
   <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:AF13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:AF6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -795,7 +796,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -893,7 +894,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -991,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1089,7 +1090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1187,203 +1188,203 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="C6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="D6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="E6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="F6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="G6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="H6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="I6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="J6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="K6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="L6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="M6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="N6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="O6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="P6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="Q6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="R6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="S6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="T6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="U6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="V6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="W6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="X6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="Y6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="Z6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="AA6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="AB6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="AC6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="AD6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="AE6">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="AF6">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.45">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AF7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1481,7 +1482,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1579,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1677,7 +1678,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1775,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1873,7 +1874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1971,105 +1972,105 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="J14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="K14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="L14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="M14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="N14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="O14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="P14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="Q14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="R14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="S14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="T14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="U14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="V14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="W14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="X14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="Y14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="Z14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="AA14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="AB14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="AC14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="AD14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="AE14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="AF14">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2167,7 +2168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2265,7 +2266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>

</xml_diff>